<commit_message>
updated based on meeting
</commit_message>
<xml_diff>
--- a/docs/ws2/ws2_taskCompletion.xlsx
+++ b/docs/ws2/ws2_taskCompletion.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Majid\Desktop\Github-Projects\co2015-group-06-repo\docs\ws2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="335" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="335"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -86,11 +90,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -99,22 +100,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -137,7 +123,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -145,53 +131,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -250,33 +202,307 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.3302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1581395348837"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="20"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.50697674418605"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.9953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.6651162790698"/>
+    <col min="1" max="2" width="18.375"/>
+    <col min="3" max="3" width="23.125"/>
+    <col min="4" max="10" width="20"/>
+    <col min="11" max="11" width="5.5"/>
+    <col min="12" max="12" width="23"/>
+    <col min="13" max="1025" width="10.625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -292,7 +518,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -308,31 +534,31 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -340,251 +566,251 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>50</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>50</v>
       </c>
-      <c r="K4" s="1" t="n">
-        <f aca="false">SUM(C4:J4)</f>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K12" si="0">SUM(C4:J4)</f>
         <v>100</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f aca="false">IF(K4&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" ref="L4:L12" si="1">IF(K4&lt;&gt;100, "The total must equal 100%","")</f>
         <v/>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>5</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <f aca="false">SUM(C5:J5)</f>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L5" s="1" t="str">
-        <f aca="false">IF(K5&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6">
         <v>23</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>21</v>
+      </c>
+      <c r="J6">
         <v>16</v>
       </c>
-      <c r="K6" s="1" t="n">
-        <f aca="false">SUM(C6:J6)</f>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L6" s="1" t="str">
-        <f aca="false">IF(K6&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>15</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+      <c r="J7">
         <v>20</v>
       </c>
-      <c r="K7" s="1" t="n">
-        <f aca="false">SUM(C7:J7)</f>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L7" s="1" t="str">
-        <f aca="false">IF(K7&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>9</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K8" s="1" t="n">
-        <f aca="false">SUM(C8:J8)</f>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f aca="false">IF(K8&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>75</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9">
         <v>25</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <f aca="false">SUM(C9:J9)</f>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f aca="false">IF(K9&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K10" s="1" t="n">
-        <f aca="false">SUM(C10:J10)</f>
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f aca="false">IF(K10&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="K11" s="1" t="n">
-        <f aca="false">SUM(C11:J11)</f>
+      <c r="C11">
+        <v>42</v>
+      </c>
+      <c r="H11">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f aca="false">IF(K11&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>18</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>50</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>50</v>
       </c>
-      <c r="K12" s="1" t="n">
-        <f aca="false">SUM(C12:J12)</f>
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f aca="false">IF(K12&lt;&gt;100, "The total must equal 100%","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1" t="n">
-        <f aca="false">$B4*C4/100+$B5*C5/100+$B6*C6/100+$B7*C7/100+$B8*C8/100+$B9*C9/100+$B10*C10/100+$B11*C11/100+$B12*C12/100</f>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:J13" si="2">$B4*C4/100+$B5*C5/100+$B6*C6/100+$B7*C7/100+$B8*C8/100+$B9*C9/100+$B10*C10/100+$B11*C11/100+$B12*C12/100</f>
+        <v>12.6</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
         <v>12.45</v>
       </c>
-      <c r="D13" s="1" t="n">
-        <f aca="false">$B4*D4/100+$B5*D5/100+$B6*D6/100+$B7*D7/100+$B8*D8/100+$B9*D9/100+$B10*D10/100+$B11*D11/100+$B12*D12/100</f>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>12.6</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
         <v>12.45</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <f aca="false">$B4*E4/100+$B5*E5/100+$B6*E6/100+$B7*E7/100+$B8*E8/100+$B9*E9/100+$B10*E10/100+$B11*E11/100+$B12*E12/100</f>
-        <v>12.5</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <f aca="false">$B4*F4/100+$B5*F5/100+$B6*F6/100+$B7*F7/100+$B8*F8/100+$B9*F9/100+$B10*F10/100+$B11*F11/100+$B12*F12/100</f>
-        <v>12.5</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <f aca="false">$B4*G4/100+$B5*G5/100+$B6*G6/100+$B7*G7/100+$B8*G8/100+$B9*G9/100+$B10*G10/100+$B11*G11/100+$B12*G12/100</f>
-        <v>12.5</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <f aca="false">$B4*H4/100+$B5*H5/100+$B6*H6/100+$B7*H7/100+$B8*H8/100+$B9*H9/100+$B10*H10/100+$B11*H11/100+$B12*H12/100</f>
-        <v>12.6</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <f aca="false">$B4*I4/100+$B5*I5/100+$B6*I6/100+$B7*I7/100+$B8*I8/100+$B9*I9/100+$B10*I10/100+$B11*I11/100+$B12*I12/100</f>
-        <v>12.6</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <f aca="false">$B4*J4/100+$B5*J5/100+$B6*J6/100+$B7*J7/100+$B8*J8/100+$B9*J9/100+$B10*J10/100+$B11*J11/100+$B12*J12/100</f>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
         <v>12.4</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -598,56 +824,51 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <f aca="false">COUNTA(C3:J3)</f>
+      <c r="B15" s="1">
+        <f>COUNTA(C3:J3)</f>
         <v>8</v>
       </c>
       <c r="C15" s="1" t="str">
-        <f aca="false">IF(C13&lt;((100/$B$15)-0.2),"you may get low marks",IF(C13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" ref="C15:J15" si="3">IF(C13&lt;((100/$B$15)-0.2),"you may get low marks",IF(C13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
         <v>fair allocation</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f aca="false">IF(D13&lt;((100/$B$15)-0.2),"you may get low marks",IF(D13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f aca="false">IF(E13&lt;((100/$B$15)-0.2),"you may get low marks",IF(E13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f aca="false">IF(F13&lt;((100/$B$15)-0.2),"you may get low marks",IF(F13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f aca="false">IF(G13&lt;((100/$B$15)-0.2),"you may get low marks",IF(G13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f aca="false">IF(H13&lt;((100/$B$15)-0.2),"you may get low marks",IF(H13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f aca="false">IF(I13&lt;((100/$B$15)-0.2),"you may get low marks",IF(I13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f aca="false">IF(J13&lt;((100/$B$15)-0.2),"you may get low marks",IF(J13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
+        <f t="shared" si="3"/>
         <v>fair allocation</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated task allocation sheet
</commit_message>
<xml_diff>
--- a/docs/ws2/ws2_taskCompletion.xlsx
+++ b/docs/ws2/ws2_taskCompletion.xlsx
@@ -97,6 +97,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -119,6 +120,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -375,9 +377,11 @@
         <f aca="false">SUM(C5:J5)</f>
         <v>100</v>
       </c>
-      <c r="L5" s="1" t="str">
+      <c r="L5" s="1" t="inlineStr">
         <f aca="false">IF(K5&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,9 +410,11 @@
         <f aca="false">SUM(C6:J6)</f>
         <v>100</v>
       </c>
-      <c r="L6" s="1" t="str">
+      <c r="L6" s="1" t="inlineStr">
         <f aca="false">IF(K6&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,9 +437,11 @@
         <f aca="false">SUM(C7:J7)</f>
         <v>100</v>
       </c>
-      <c r="L7" s="1" t="str">
+      <c r="L7" s="1" t="inlineStr">
         <f aca="false">IF(K7&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,9 +458,11 @@
         <f aca="false">SUM(C8:J8)</f>
         <v>100</v>
       </c>
-      <c r="L8" s="1" t="str">
+      <c r="L8" s="1" t="inlineStr">
         <f aca="false">IF(K8&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,9 +482,11 @@
         <f aca="false">SUM(C9:J9)</f>
         <v>100</v>
       </c>
-      <c r="L9" s="1" t="str">
+      <c r="L9" s="1" t="inlineStr">
         <f aca="false">IF(K9&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,9 +503,11 @@
         <f aca="false">SUM(C10:J10)</f>
         <v>100</v>
       </c>
-      <c r="L10" s="1" t="str">
+      <c r="L10" s="1" t="inlineStr">
         <f aca="false">IF(K10&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,9 +530,11 @@
         <f aca="false">SUM(C11:J11)</f>
         <v>100</v>
       </c>
-      <c r="L11" s="1" t="str">
+      <c r="L11" s="1" t="inlineStr">
         <f aca="false">IF(K11&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,9 +554,11 @@
         <f aca="false">SUM(C12:J12)</f>
         <v>100</v>
       </c>
-      <c r="L12" s="1" t="str">
+      <c r="L12" s="1" t="inlineStr">
         <f aca="false">IF(K12&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,7 +682,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -781,9 +799,11 @@
         <f aca="false">SUM(C5:J5)</f>
         <v>100</v>
       </c>
-      <c r="L5" s="1" t="str">
+      <c r="L5" s="1" t="inlineStr">
         <f aca="false">IF(K5&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,19 +814,19 @@
         <v>15</v>
       </c>
       <c r="D6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>25</v>
-      </c>
       <c r="I6" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1" t="n">
         <f aca="false">SUM(C6:J6)</f>
@@ -834,9 +854,11 @@
         <f aca="false">SUM(C7:J7)</f>
         <v>100</v>
       </c>
-      <c r="L7" s="1" t="str">
+      <c r="L7" s="1" t="inlineStr">
         <f aca="false">IF(K7&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,9 +875,11 @@
         <f aca="false">SUM(C8:J8)</f>
         <v>100</v>
       </c>
-      <c r="L8" s="1" t="str">
+      <c r="L8" s="1" t="inlineStr">
         <f aca="false">IF(K8&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,9 +899,11 @@
         <f aca="false">SUM(C9:J9)</f>
         <v>100</v>
       </c>
-      <c r="L9" s="1" t="str">
+      <c r="L9" s="1" t="inlineStr">
         <f aca="false">IF(K9&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,9 +923,11 @@
         <f aca="false">SUM(C10:J10)</f>
         <v>100</v>
       </c>
-      <c r="L10" s="1" t="str">
+      <c r="L10" s="1" t="inlineStr">
         <f aca="false">IF(K10&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,9 +950,11 @@
         <f aca="false">SUM(C11:J11)</f>
         <v>100</v>
       </c>
-      <c r="L11" s="1" t="str">
+      <c r="L11" s="1" t="inlineStr">
         <f aca="false">IF(K11&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,9 +989,11 @@
         <f aca="false">SUM(C12:J12)</f>
         <v>100</v>
       </c>
-      <c r="L12" s="1" t="str">
+      <c r="L12" s="1" t="inlineStr">
         <f aca="false">IF(K12&lt;&gt;100, "The total must equal 100%","")</f>
-        <v/>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,19 +1007,19 @@
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">$B4*D4/100+$B5*D5/100+$B6*D6/100+$B7*D7/100+$B8*D8/100+$B9*D9/100+$B10*D10/100+$B11*D11/100+$B12*D12/100</f>
-        <v>13.8</v>
+        <v>13.05</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">$B4*E4/100+$B5*E5/100+$B6*E6/100+$B7*E7/100+$B8*E8/100+$B9*E9/100+$B10*E10/100+$B11*E11/100+$B12*E12/100</f>
-        <v>13.4</v>
+        <v>12.875</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">$B4*F4/100+$B5*F5/100+$B6*F6/100+$B7*F7/100+$B8*F8/100+$B9*F9/100+$B10*F10/100+$B11*F11/100+$B12*F12/100</f>
-        <v>13.55</v>
+        <v>12.575</v>
       </c>
       <c r="G13" s="1" t="n">
         <f aca="false">$B4*G4/100+$B5*G5/100+$B6*G6/100+$B7*G7/100+$B8*G8/100+$B9*G9/100+$B10*G10/100+$B11*G11/100+$B12*G12/100</f>
-        <v>14.45</v>
+        <v>13.7</v>
       </c>
       <c r="H13" s="1" t="n">
         <f aca="false">$B4*H4/100+$B5*H5/100+$B6*H6/100+$B7*H7/100+$B8*H8/100+$B9*H9/100+$B10*H10/100+$B11*H11/100+$B12*H12/100</f>
@@ -995,7 +1027,7 @@
       </c>
       <c r="I13" s="1" t="n">
         <f aca="false">$B4*I4/100+$B5*I5/100+$B6*I6/100+$B7*I7/100+$B8*I8/100+$B9*I9/100+$B10*I10/100+$B11*I11/100+$B12*I12/100</f>
-        <v>15.8</v>
+        <v>18.8</v>
       </c>
       <c r="J13" s="1" t="n">
         <f aca="false">$B4*J4/100+$B5*J5/100+$B6*J6/100+$B7*J7/100+$B8*J8/100+$B9*J9/100+$B10*J10/100+$B11*J11/100+$B12*J12/100</f>
@@ -1040,7 +1072,7 @@
       </c>
       <c r="F15" s="1" t="str">
         <f aca="false">IF(F13&lt;((100/$B$15)-0.2),"you may get low marks",IF(F13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>
-        <v>you are doing too much</v>
+        <v>fair allocation</v>
       </c>
       <c r="G15" s="1" t="str">
         <f aca="false">IF(G13&lt;((100/$B$15)-0.2),"you may get low marks",IF(G13&gt;((100/$B$15)+0.2),"you are doing too much","fair allocation"))</f>

</xml_diff>